<commit_message>
Country report script updated
</commit_message>
<xml_diff>
--- a/Inputs/IATI returns/MODARI award data - GHS (GAMRIF and UKVN).xlsx
+++ b/Inputs/IATI returns/MODARI award data - GHS (GAMRIF and UKVN).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/IATI returns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{E4CC7446-E93A-46D5-86D9-2234D76FE536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{0FEC7A05-FC5C-4E3C-926A-FD65731D1C5A}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{E4CC7446-E93A-46D5-86D9-2234D76FE536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{A9FC78CA-E064-4160-A170-A3B1D7B4AB8B}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4496,10 +4496,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4592,7 +4593,7 @@
       <c r="W1" s="9"/>
       <c r="X1" s="9"/>
     </row>
-    <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -4654,7 +4655,7 @@
       <c r="W2" s="13"/>
       <c r="X2" s="13"/>
     </row>
-    <row r="3" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -4716,7 +4717,7 @@
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
     </row>
-    <row r="4" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -4778,7 +4779,7 @@
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -4840,7 +4841,7 @@
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -4902,7 +4903,7 @@
       <c r="W6" s="13"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -4964,7 +4965,7 @@
       <c r="W7" s="13"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -5026,7 +5027,7 @@
       <c r="W8" s="13"/>
       <c r="X8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -5088,7 +5089,7 @@
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
     </row>
-    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -5150,7 +5151,7 @@
       <c r="W10" s="13"/>
       <c r="X10" s="13"/>
     </row>
-    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>10</v>
       </c>
@@ -5212,7 +5213,7 @@
       <c r="W11" s="13"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <v>11</v>
       </c>
@@ -5274,7 +5275,7 @@
       <c r="W12" s="13"/>
       <c r="X12" s="13"/>
     </row>
-    <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -5336,7 +5337,7 @@
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
     </row>
-    <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -5398,7 +5399,7 @@
       <c r="W14" s="13"/>
       <c r="X14" s="13"/>
     </row>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -5460,7 +5461,7 @@
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
     </row>
-    <row r="16" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -5512,7 +5513,7 @@
       <c r="W16" s="13"/>
       <c r="X16" s="13"/>
     </row>
-    <row r="17" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -5564,7 +5565,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -5616,7 +5617,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>18</v>
       </c>
@@ -5668,7 +5669,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>19</v>
       </c>
@@ -5720,7 +5721,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -5772,7 +5773,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18">
         <v>21</v>
       </c>
@@ -5830,7 +5831,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>22</v>
       </c>
@@ -5888,7 +5889,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18">
         <v>23</v>
       </c>
@@ -5946,7 +5947,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <v>24</v>
       </c>
@@ -6004,7 +6005,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18">
         <v>25</v>
       </c>
@@ -6062,7 +6063,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18">
         <v>26</v>
       </c>
@@ -6118,7 +6119,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18">
         <v>27</v>
       </c>
@@ -6176,7 +6177,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
         <v>28</v>
       </c>
@@ -6234,7 +6235,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18">
         <v>29</v>
       </c>
@@ -6292,7 +6293,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18">
         <v>30</v>
       </c>
@@ -6350,7 +6351,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18">
         <v>31</v>
       </c>
@@ -6718,7 +6719,7 @@
       <c r="W37" s="13"/>
       <c r="X37" s="13"/>
     </row>
-    <row r="38" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="18">
         <v>37</v>
       </c>
@@ -6774,7 +6775,7 @@
       <c r="W38" s="14"/>
       <c r="X38" s="14"/>
     </row>
-    <row r="39" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18">
         <v>38</v>
       </c>
@@ -6830,7 +6831,7 @@
       <c r="W39" s="14"/>
       <c r="X39" s="14"/>
     </row>
-    <row r="40" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18">
         <v>39</v>
       </c>
@@ -6886,7 +6887,7 @@
       <c r="W40" s="14"/>
       <c r="X40" s="14"/>
     </row>
-    <row r="41" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18">
         <v>40</v>
       </c>
@@ -6942,7 +6943,7 @@
       <c r="W41" s="14"/>
       <c r="X41" s="14"/>
     </row>
-    <row r="42" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
         <v>41</v>
       </c>
@@ -6998,7 +6999,7 @@
       <c r="W42" s="14"/>
       <c r="X42" s="14"/>
     </row>
-    <row r="43" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
         <v>42</v>
       </c>
@@ -7060,7 +7061,7 @@
       <c r="W43" s="14"/>
       <c r="X43" s="14"/>
     </row>
-    <row r="44" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18">
         <v>43</v>
       </c>
@@ -7122,7 +7123,7 @@
       <c r="W44" s="14"/>
       <c r="X44" s="14"/>
     </row>
-    <row r="45" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18">
         <v>44</v>
       </c>
@@ -7184,7 +7185,7 @@
       <c r="W45" s="13"/>
       <c r="X45" s="13"/>
     </row>
-    <row r="46" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18">
         <v>45</v>
       </c>
@@ -7246,7 +7247,7 @@
       <c r="W46" s="13"/>
       <c r="X46" s="13"/>
     </row>
-    <row r="47" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18">
         <v>46</v>
       </c>
@@ -7308,7 +7309,7 @@
       <c r="W47" s="13"/>
       <c r="X47" s="13"/>
     </row>
-    <row r="48" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18">
         <v>47</v>
       </c>
@@ -7370,7 +7371,7 @@
       <c r="W48" s="13"/>
       <c r="X48" s="13"/>
     </row>
-    <row r="49" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18">
         <v>48</v>
       </c>
@@ -7428,7 +7429,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18">
         <v>49</v>
       </c>
@@ -7486,7 +7487,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18">
         <v>50</v>
       </c>
@@ -7544,7 +7545,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
         <v>51</v>
       </c>
@@ -7602,7 +7603,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18">
         <v>52</v>
       </c>
@@ -7660,7 +7661,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18">
         <v>53</v>
       </c>
@@ -7716,7 +7717,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="18">
         <v>54</v>
       </c>
@@ -7774,7 +7775,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="18">
         <v>55</v>
       </c>
@@ -7832,7 +7833,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="18">
         <v>56</v>
       </c>
@@ -7890,7 +7891,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18">
         <v>57</v>
       </c>
@@ -7948,7 +7949,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18">
         <v>58</v>
       </c>
@@ -8006,7 +8007,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18">
         <v>59</v>
       </c>
@@ -8060,7 +8061,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="18">
         <v>60</v>
       </c>
@@ -8112,7 +8113,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18">
         <v>61</v>
       </c>
@@ -8164,7 +8165,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18">
         <v>62</v>
       </c>
@@ -8216,7 +8217,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="18">
         <v>63</v>
       </c>
@@ -8270,7 +8271,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18">
         <v>64</v>
       </c>
@@ -8324,7 +8325,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="18">
         <v>65</v>
       </c>
@@ -8376,7 +8377,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="18">
         <v>66</v>
       </c>
@@ -8430,7 +8431,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18">
         <v>67</v>
       </c>
@@ -8482,7 +8483,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18">
         <v>68</v>
       </c>
@@ -8534,7 +8535,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="18">
         <v>69</v>
       </c>
@@ -8588,7 +8589,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="18">
         <v>70</v>
       </c>
@@ -8640,7 +8641,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="18">
         <v>71</v>
       </c>
@@ -8692,7 +8693,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="18">
         <v>72</v>
       </c>
@@ -8746,7 +8747,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="18">
         <v>73</v>
       </c>
@@ -8802,7 +8803,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="18">
         <v>74</v>
       </c>
@@ -8854,7 +8855,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="18">
         <v>75</v>
       </c>
@@ -8906,7 +8907,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="18">
         <v>76</v>
       </c>
@@ -8960,7 +8961,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="18">
         <v>77</v>
       </c>
@@ -9014,7 +9015,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="18">
         <v>78</v>
       </c>
@@ -9068,7 +9069,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="18">
         <v>79</v>
       </c>
@@ -9120,7 +9121,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="18">
         <v>80</v>
       </c>
@@ -9172,7 +9173,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="18">
         <v>81</v>
       </c>
@@ -9224,7 +9225,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="18">
         <v>82</v>
       </c>
@@ -9276,7 +9277,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="18">
         <v>83</v>
       </c>
@@ -9324,7 +9325,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="18">
         <v>84</v>
       </c>
@@ -9372,7 +9373,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="18">
         <v>85</v>
       </c>
@@ -9420,7 +9421,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="18">
         <v>86</v>
       </c>
@@ -9468,7 +9469,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="18">
         <v>87</v>
       </c>
@@ -9516,7 +9517,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="18">
         <v>88</v>
       </c>
@@ -9562,7 +9563,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="18">
         <v>89</v>
       </c>
@@ -9620,7 +9621,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="18">
         <v>90</v>
       </c>
@@ -9678,7 +9679,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="18">
         <v>91</v>
       </c>
@@ -9730,7 +9731,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="18">
         <v>92</v>
       </c>
@@ -9784,7 +9785,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="18">
         <v>93</v>
       </c>
@@ -9838,7 +9839,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="18">
         <v>94</v>
       </c>
@@ -9890,7 +9891,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="18">
         <v>95</v>
       </c>
@@ -9942,7 +9943,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="18">
         <v>96</v>
       </c>
@@ -9996,7 +9997,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="18">
         <v>97</v>
       </c>
@@ -10050,7 +10051,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="18">
         <v>98</v>
       </c>
@@ -10108,7 +10109,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="18">
         <v>99</v>
       </c>
@@ -10162,7 +10163,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="18">
         <v>100</v>
       </c>
@@ -10216,7 +10217,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="18">
         <v>101</v>
       </c>
@@ -10274,7 +10275,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="18">
         <v>102</v>
       </c>
@@ -10328,7 +10329,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="18">
         <v>103</v>
       </c>
@@ -10382,7 +10383,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="18">
         <v>104</v>
       </c>
@@ -10440,7 +10441,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="18">
         <v>105</v>
       </c>
@@ -10492,7 +10493,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="18">
         <v>106</v>
       </c>
@@ -10544,7 +10545,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="18">
         <v>107</v>
       </c>
@@ -10598,7 +10599,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="18">
         <v>108</v>
       </c>
@@ -10650,7 +10651,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="18">
         <v>109</v>
       </c>
@@ -10704,7 +10705,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="18">
         <v>110</v>
       </c>
@@ -10758,7 +10759,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="18">
         <v>111</v>
       </c>
@@ -10810,7 +10811,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="18">
         <v>112</v>
       </c>
@@ -10864,7 +10865,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="18">
         <v>113</v>
       </c>
@@ -10918,7 +10919,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="18">
         <v>114</v>
       </c>
@@ -10972,7 +10973,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="18">
         <v>115</v>
       </c>
@@ -11026,7 +11027,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="18">
         <v>116</v>
       </c>
@@ -11080,7 +11081,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="18">
         <v>117</v>
       </c>
@@ -11134,7 +11135,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="18">
         <v>118</v>
       </c>
@@ -11186,7 +11187,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="18">
         <v>119</v>
       </c>
@@ -11240,7 +11241,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="18">
         <v>120</v>
       </c>
@@ -11294,7 +11295,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="18">
         <v>121</v>
       </c>
@@ -11348,7 +11349,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="18">
         <v>122</v>
       </c>
@@ -11400,7 +11401,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="18">
         <v>123</v>
       </c>
@@ -11454,7 +11455,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="18">
         <v>124</v>
       </c>
@@ -11914,7 +11915,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="18">
         <v>132</v>
       </c>
@@ -11964,7 +11965,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="18">
         <v>133</v>
       </c>
@@ -12014,7 +12015,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="18">
         <v>134</v>
       </c>
@@ -12064,7 +12065,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="18">
         <v>135</v>
       </c>
@@ -12114,7 +12115,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="18">
         <v>136</v>
       </c>
@@ -30369,12 +30370,29 @@
       <c r="T1000" s="11"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:T137" xr:uid="{202AB705-7DF7-4EB4-9C34-ED7EC588D9EA}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="BBSRC"/>
+        <filter val="EPSRC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6713CC7F31D7C498DF06765AF1263E4" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="366367cd6cb5cdab93a9cfb77f1d8fd4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="9e449739-2858-4f41-8e5c-7dc6df20853e" xmlns:ns4="05c15269-663a-4da2-bb2b-1510839404b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bea9f5ec70232b46c2a1df78798852fa" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -30614,15 +30632,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -30633,6 +30642,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3C49041-F246-4B03-A83A-30F6FFFE0FD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDF78AE5-A260-457C-8C49-38550BF821A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30652,16 +30671,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3C49041-F246-4B03-A83A-30F6FFFE0FD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D95885E-3D3E-41C7-BCB5-60294B0AB1EE}">
   <ds:schemaRefs>

</xml_diff>